<commit_message>
beginning to work on apps
</commit_message>
<xml_diff>
--- a/mock_data.xlsx
+++ b/mock_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Narozzy-GitHub\AutoNiner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A844E0-1E5C-43B9-970A-A3E544567911}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3745FB1-F6F4-419A-A230-93C1D731A7B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7275" yWindow="1605" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -378,7 +378,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>